<commit_message>
[gebgl-360]  Inmersive navigation. [marilolis]  Marilolis qr redirection
</commit_message>
<xml_diff>
--- a/contabilidad/contabilidad-casa.xlsx
+++ b/contabilidad/contabilidad-casa.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ruben\personal\amigos\cristina\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\work_seas\pfm_vimo-presentacion\0dr4d3k.github.io\contabilidad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9F3B539E-538B-47F3-ADC2-6A118EE81CF0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{539F2F6F-EED2-4DE3-8447-9A9304B6ED58}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{A4F8636C-2B19-4617-A987-A143781C94F5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{A4F8636C-2B19-4617-A987-A143781C94F5}"/>
   </bookViews>
   <sheets>
     <sheet name="Gastos Cristian-Cristina-Ruben" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="20">
   <si>
     <t>Cristina</t>
   </si>
@@ -89,13 +89,19 @@
   <si>
     <t>internet</t>
   </si>
+  <si>
+    <t>indicar fecha</t>
+  </si>
+  <si>
+    <t>indicar gasto</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="#,##0.00\ &quot;€&quot;"/>
+    <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -173,22 +179,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -197,12 +204,94 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="47">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -235,6 +324,16 @@
     </dxf>
     <dxf>
       <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -265,6 +364,11 @@
     </dxf>
     <dxf>
       <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -275,6 +379,50 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -304,46 +452,44 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="166" formatCode="#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -362,11 +508,11 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{3807380F-C9A1-4EC0-A14D-A892F69CB9D9}" name="Tabla25" displayName="Tabla25" ref="B3:F24" totalsRowShown="0">
   <autoFilter ref="B3:F24" xr:uid="{1AF39082-7A53-4315-B89E-81D93BF6ECCE}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{40E90C76-2F1C-4BE4-95B8-BDECFEAFCC98}" name="Fecha" dataDxfId="23"/>
-    <tableColumn id="2" xr3:uid="{10CB6F76-F204-42A7-B0E9-86B897511552}" name="Tipo"/>
-    <tableColumn id="3" xr3:uid="{6CF439CE-2FBB-43C7-A80E-BF561F805CF8}" name="Cristian" dataDxfId="17"/>
-    <tableColumn id="4" xr3:uid="{94EE4FDC-183E-45D3-AEB7-CA124A6AA2CD}" name="Cristina" dataDxfId="16"/>
-    <tableColumn id="5" xr3:uid="{D2F7ADC0-7CAA-422D-BB30-2F5CEF984BD4}" name="Ruben" dataDxfId="15"/>
+    <tableColumn id="1" xr3:uid="{40E90C76-2F1C-4BE4-95B8-BDECFEAFCC98}" name="Fecha" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{10CB6F76-F204-42A7-B0E9-86B897511552}" name="Tipo" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{6CF439CE-2FBB-43C7-A80E-BF561F805CF8}" name="Cristian" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{94EE4FDC-183E-45D3-AEB7-CA124A6AA2CD}" name="Cristina" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{D2F7ADC0-7CAA-422D-BB30-2F5CEF984BD4}" name="Ruben" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -376,10 +522,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{136D32F1-BBE8-4F0F-8E78-8C3C96CE3C97}" name="Tabla2611" displayName="Tabla2611" ref="B3:E24" totalsRowShown="0">
   <autoFilter ref="B3:E24" xr:uid="{7E9D333B-3422-429E-8D90-7D21C20F26ED}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{01F6EDF6-6F1A-4135-8FB2-B2E189DD11B8}" name="Fecha" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{4EA8AF4E-826C-4860-BF5F-9195D478B927}" name="Tipo"/>
-    <tableColumn id="3" xr3:uid="{7017F726-29F6-4B9A-8A2C-E648D490179C}" name="Cristian" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{62527E48-3571-480C-AB47-873CB4544825}" name="Cristina" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{01F6EDF6-6F1A-4135-8FB2-B2E189DD11B8}" name="Fecha" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{4EA8AF4E-826C-4860-BF5F-9195D478B927}" name="Tipo" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{7017F726-29F6-4B9A-8A2C-E648D490179C}" name="Cristian" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{62527E48-3571-480C-AB47-873CB4544825}" name="Cristina" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -389,10 +535,14 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{0E659316-BB14-4DD4-9C3D-C48B96835DB9}" name="Tabla26" displayName="Tabla26" ref="B3:E24" totalsRowShown="0">
   <autoFilter ref="B3:E24" xr:uid="{7E9D333B-3422-429E-8D90-7D21C20F26ED}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{9E56747A-7F6D-4A8E-AB42-E835C5865B72}" name="Fecha" dataDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{7F32AC0A-ACBA-4DE8-BF48-3E2297E44B03}" name="Tipo"/>
-    <tableColumn id="3" xr3:uid="{13BA8E98-3DD0-49F5-B49F-6DBE3CC44BB5}" name="Cristina" dataDxfId="21"/>
-    <tableColumn id="4" xr3:uid="{4FD13738-44B6-4174-8475-6431FDEFF0DD}" name="Ruben" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{9E56747A-7F6D-4A8E-AB42-E835C5865B72}" name="Fecha" dataDxfId="34"/>
+    <tableColumn id="2" xr3:uid="{7F32AC0A-ACBA-4DE8-BF48-3E2297E44B03}" name="Tipo" dataDxfId="32"/>
+    <tableColumn id="3" xr3:uid="{13BA8E98-3DD0-49F5-B49F-6DBE3CC44BB5}" name="Cristina" dataDxfId="33">
+      <calculatedColumnFormula>IF(D4="",0)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{4FD13738-44B6-4174-8475-6431FDEFF0DD}" name="Ruben" dataDxfId="35">
+      <calculatedColumnFormula>IF(E4="",0)</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -402,13 +552,13 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{A0F033CE-88C8-4955-9B7A-BF1E7497C9C3}" name="Tabla2510" displayName="Tabla2510" ref="B3:F6" totalsRowShown="0">
   <autoFilter ref="B3:F6" xr:uid="{96647A87-E06D-49D3-B088-ABFFFA7DDCAF}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{40CA2073-99F3-443E-BDFC-9A99BDD26596}" name="Fecha" dataDxfId="19"/>
+    <tableColumn id="1" xr3:uid="{40CA2073-99F3-443E-BDFC-9A99BDD26596}" name="Fecha" dataDxfId="39"/>
     <tableColumn id="2" xr3:uid="{D065263B-BC39-48B8-88B0-9C4235EF8B65}" name="Tipo"/>
-    <tableColumn id="3" xr3:uid="{CD61F4FD-A33B-4A8B-A8E1-C66DC6DA3E10}" name="Cristian" dataDxfId="18"/>
-    <tableColumn id="4" xr3:uid="{CA023837-BE6C-4426-A285-6993CAB08A38}" name="Cristina" dataDxfId="14">
+    <tableColumn id="3" xr3:uid="{CD61F4FD-A33B-4A8B-A8E1-C66DC6DA3E10}" name="Cristian" dataDxfId="38"/>
+    <tableColumn id="4" xr3:uid="{CA023837-BE6C-4426-A285-6993CAB08A38}" name="Cristina" dataDxfId="37">
       <calculatedColumnFormula>'Gastos Cristina-Ruben'!D25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{82F8DF0E-0AE5-4D45-A44D-45C6EA0C5B23}" name="Ruben" dataDxfId="13">
+    <tableColumn id="5" xr3:uid="{82F8DF0E-0AE5-4D45-A44D-45C6EA0C5B23}" name="Ruben" dataDxfId="36">
       <calculatedColumnFormula>'Gastos Cristina-Ruben'!E25</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -715,8 +865,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB6D4BEA-3EE6-4DEA-97EE-8DA07141A625}">
   <dimension ref="B2:F29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -753,216 +903,430 @@
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B4" s="1"/>
-      <c r="C4" t="s">
+      <c r="B4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0</v>
+      </c>
+      <c r="E4" s="3">
+        <v>450</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B5" s="1"/>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B6" s="1"/>
-      <c r="C6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B7" s="1"/>
-      <c r="C7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B8" s="1"/>
-      <c r="C8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5">
-        <v>450</v>
-      </c>
-      <c r="F8" s="5"/>
+      <c r="D8" s="3">
+        <v>0</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B9" s="1"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
+      <c r="B9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B10" s="1"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
+      <c r="B10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0</v>
+      </c>
+      <c r="F10" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B11" s="1"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
+      <c r="B11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0</v>
+      </c>
+      <c r="F11" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B12" s="1"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
+      <c r="B12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B13" s="1"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
+      <c r="B13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0</v>
+      </c>
+      <c r="F13" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B14" s="1"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
+      <c r="B14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0</v>
+      </c>
+      <c r="E14" s="3">
+        <v>0</v>
+      </c>
+      <c r="F14" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B15" s="1"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
+      <c r="B15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="3">
+        <v>0</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0</v>
+      </c>
+      <c r="F15" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B16" s="1"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
+      <c r="B16" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="3">
+        <v>0</v>
+      </c>
+      <c r="E16" s="3">
+        <v>0</v>
+      </c>
+      <c r="F16" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B17" s="1"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
+      <c r="B17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="3">
+        <v>0</v>
+      </c>
+      <c r="E17" s="3">
+        <v>0</v>
+      </c>
+      <c r="F17" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B18" s="1"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
+      <c r="B18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="3">
+        <v>0</v>
+      </c>
+      <c r="E18" s="3">
+        <v>0</v>
+      </c>
+      <c r="F18" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B19" s="1"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
+      <c r="B19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="3">
+        <v>0</v>
+      </c>
+      <c r="E19" s="3">
+        <v>0</v>
+      </c>
+      <c r="F19" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B20" s="1"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
+      <c r="B20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" s="3">
+        <v>0</v>
+      </c>
+      <c r="E20" s="3">
+        <v>0</v>
+      </c>
+      <c r="F20" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B21" s="1"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
+      <c r="B21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" s="3">
+        <v>0</v>
+      </c>
+      <c r="E21" s="3">
+        <v>0</v>
+      </c>
+      <c r="F21" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B22" s="1"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
+      <c r="B22" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" s="3">
+        <v>0</v>
+      </c>
+      <c r="E22" s="3">
+        <v>0</v>
+      </c>
+      <c r="F22" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B23" s="1"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
+      <c r="B23" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" s="3">
+        <v>0</v>
+      </c>
+      <c r="E23" s="3">
+        <v>0</v>
+      </c>
+      <c r="F23" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B24" s="1"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
+      <c r="B24" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D24" s="3">
+        <v>0</v>
+      </c>
+      <c r="E24" s="3">
+        <v>0</v>
+      </c>
+      <c r="F24" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="26" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C26" s="4"/>
-      <c r="D26" s="6">
+      <c r="C26" s="7"/>
+      <c r="D26" s="4">
         <f>SUM(D4:D23)</f>
         <v>0</v>
       </c>
-      <c r="E26" s="6">
+      <c r="E26" s="4">
         <f>SUM(E4:E23)</f>
         <v>450</v>
       </c>
-      <c r="F26" s="6">
-        <f t="shared" ref="E26:F26" si="0">SUM(F4:F23)</f>
+      <c r="F26" s="4">
+        <f t="shared" ref="F26" si="0">SUM(F4:F23)</f>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C27" s="4"/>
-      <c r="D27" s="6">
+      <c r="C27" s="7"/>
+      <c r="D27" s="4">
         <f>(D26+E26+F26)/3</f>
         <v>150</v>
       </c>
-      <c r="E27" s="6">
+      <c r="E27" s="4">
         <f>(D26+E26+F26)/3</f>
         <v>150</v>
       </c>
-      <c r="F27" s="6">
+      <c r="F27" s="4">
         <f>(D26+E26+F26)/3</f>
         <v>150</v>
       </c>
     </row>
     <row r="28" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B28" s="3"/>
-      <c r="C28" s="7" t="s">
+      <c r="B28" s="2"/>
+      <c r="C28" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D28" s="6">
+      <c r="D28" s="4">
         <f>IF((D27-D26) &lt;= 0, 0, (D27-D26))</f>
         <v>150</v>
       </c>
-      <c r="E28" s="6">
+      <c r="E28" s="4">
         <f t="shared" ref="E28:F28" si="1">IF((E27-E26) &lt;= 0, 0, (E27-E26))</f>
         <v>0</v>
       </c>
-      <c r="F28" s="6">
+      <c r="F28" s="4">
         <f t="shared" si="1"/>
         <v>150</v>
       </c>
     </row>
     <row r="29" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B29" s="3"/>
-      <c r="C29" s="7" t="s">
+      <c r="B29" s="2"/>
+      <c r="C29" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D29" s="6">
+      <c r="D29" s="4">
         <f>IF((D27-D26) &lt;= 0, (D26-D27), 0 )</f>
         <v>0</v>
       </c>
-      <c r="E29" s="6">
+      <c r="E29" s="4">
         <f>IF((E27-E26) &lt;= 0, (E26-E27), 0 )</f>
         <v>300</v>
       </c>
-      <c r="F29" s="6">
+      <c r="F29" s="4">
         <f>IF((F27-F26) &lt;= 0, (F26-F27), 0 )</f>
         <v>0</v>
       </c>
@@ -974,23 +1338,48 @@
     <mergeCell ref="B2:F2"/>
   </mergeCells>
   <conditionalFormatting sqref="D28:F28">
-    <cfRule type="cellIs" dxfId="9" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="46" priority="10" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D28:F28">
-    <cfRule type="cellIs" dxfId="8" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="45" priority="9" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D29:E29">
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="44" priority="8" operator="greaterThan">
       <formula>18.55</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F29">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="43" priority="6" operator="greaterThan">
       <formula>18.55</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4:B24">
+    <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
+      <formula>"indicar fecha"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C4:C24">
+    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
+      <formula>"indicar gasto"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D4:D24">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E4:E24">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F4:F24">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1006,7 +1395,7 @@
   <dimension ref="B2:E29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:E24"/>
+      <selection activeCell="D4" sqref="D4:D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1017,12 +1406,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
@@ -1039,162 +1428,351 @@
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B4" s="1"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
+      <c r="B4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B5" s="1"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
+      <c r="B5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B6" s="1"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
+      <c r="B6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B7" s="1"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
+      <c r="B7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B8" s="1"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
+      <c r="B8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B9" s="1"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
+      <c r="B9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B10" s="1"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
+      <c r="B10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B11" s="1"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
+      <c r="B11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B12" s="1"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
+      <c r="B12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B13" s="1"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
+      <c r="B13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B14" s="1"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
+      <c r="B14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0</v>
+      </c>
+      <c r="E14" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B15" s="1"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
+      <c r="B15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="3">
+        <v>0</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B16" s="1"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
+      <c r="B16" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="3">
+        <v>0</v>
+      </c>
+      <c r="E16" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B17" s="1"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
+      <c r="B17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="3">
+        <v>0</v>
+      </c>
+      <c r="E17" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B18" s="1"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
+      <c r="B18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="3">
+        <v>0</v>
+      </c>
+      <c r="E18" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B19" s="1"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
+      <c r="B19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="3">
+        <v>0</v>
+      </c>
+      <c r="E19" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B20" s="1"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
+      <c r="B20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" s="3">
+        <v>0</v>
+      </c>
+      <c r="E20" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B21" s="1"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
+      <c r="B21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" s="3">
+        <v>0</v>
+      </c>
+      <c r="E21" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B22" s="1"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
+      <c r="B22" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" s="3">
+        <v>0</v>
+      </c>
+      <c r="E22" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B23" s="1"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
+      <c r="B23" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" s="3">
+        <v>0</v>
+      </c>
+      <c r="E23" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B24" s="1"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
+      <c r="B24" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D24" s="3">
+        <v>0</v>
+      </c>
+      <c r="E24" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="26" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C26" s="4"/>
-      <c r="D26" s="6">
+      <c r="C26" s="7"/>
+      <c r="D26" s="4">
         <f>SUM(D4:D23)</f>
         <v>0</v>
       </c>
-      <c r="E26" s="6">
+      <c r="E26" s="4">
         <f>SUM(E4:E24)</f>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C27" s="4"/>
-      <c r="D27" s="6">
+      <c r="C27" s="7"/>
+      <c r="D27" s="4">
         <f>(D26+E26)/2</f>
         <v>0</v>
       </c>
-      <c r="E27" s="6">
+      <c r="E27" s="4">
         <f>(D26+E26)/2</f>
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B28" s="3"/>
-      <c r="C28" s="7" t="s">
+      <c r="B28" s="2"/>
+      <c r="C28" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D28" s="6">
+      <c r="D28" s="4">
         <f>IF((D27-D26) &lt;= 0, 0, (D27-D26))</f>
         <v>0</v>
       </c>
-      <c r="E28" s="6">
+      <c r="E28" s="4">
         <f>IF((E27-E26) &lt;= 0, 0, (E27-E26))</f>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B29" s="3"/>
-      <c r="C29" s="7" t="s">
+      <c r="B29" s="2"/>
+      <c r="C29" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D29" s="6">
+      <c r="D29" s="4">
         <f>IF((D27-D26) &lt;= 0, (D26-D27), 0 )</f>
         <v>0</v>
       </c>
-      <c r="E29" s="6">
+      <c r="E29" s="4">
         <f>IF((E27-E26) &lt;= 0, (E26-E27), 0 )</f>
         <v>0</v>
       </c>
@@ -1206,18 +1784,33 @@
     <mergeCell ref="B27:C27"/>
   </mergeCells>
   <conditionalFormatting sqref="D28">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="42" priority="6" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D28:E28">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="41" priority="5" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D29:E29">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="40" priority="4" operator="greaterThan">
       <formula>18.55</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D4:E24">
+    <cfRule type="cellIs" dxfId="16" priority="3" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4:B24">
+    <cfRule type="cellIs" dxfId="13" priority="2" operator="equal">
+      <formula>"indicar fecha"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C4:C24">
+    <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
+      <formula>"indicar gasto"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1232,24 +1825,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AE1BA74-1E53-4E8E-B7A9-4D7765ED9DCB}">
   <dimension ref="B2:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="16.77734375" customWidth="1"/>
     <col min="3" max="3" width="17.44140625" customWidth="1"/>
-    <col min="8" max="8" width="18.21875" customWidth="1"/>
+    <col min="8" max="8" width="11.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
@@ -1266,162 +1859,351 @@
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B4" s="1"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
+      <c r="B4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B5" s="1"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
+      <c r="B5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B6" s="1"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
+      <c r="B6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B7" s="1"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
+      <c r="B7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B8" s="1"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
+      <c r="B8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B9" s="1"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
+      <c r="B9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B10" s="1"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
+      <c r="B10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B11" s="1"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
+      <c r="B11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B12" s="1"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
+      <c r="B12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B13" s="1"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
+      <c r="B13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B14" s="1"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
+      <c r="B14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0</v>
+      </c>
+      <c r="E14" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B15" s="1"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
+      <c r="B15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="3">
+        <v>0</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B16" s="1"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
+      <c r="B16" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="3">
+        <v>0</v>
+      </c>
+      <c r="E16" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B17" s="1"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
+      <c r="B17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="3">
+        <v>0</v>
+      </c>
+      <c r="E17" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B18" s="1"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
+      <c r="B18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="3">
+        <v>0</v>
+      </c>
+      <c r="E18" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B19" s="1"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
+      <c r="B19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="3">
+        <v>0</v>
+      </c>
+      <c r="E19" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B20" s="1"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
+      <c r="B20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" s="3">
+        <v>0</v>
+      </c>
+      <c r="E20" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B21" s="1"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
+      <c r="B21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" s="3">
+        <v>0</v>
+      </c>
+      <c r="E21" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B22" s="1"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
+      <c r="B22" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" s="3">
+        <v>0</v>
+      </c>
+      <c r="E22" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B23" s="1"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
+      <c r="B23" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" s="3">
+        <v>0</v>
+      </c>
+      <c r="E23" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B24" s="1"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
+      <c r="B24" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D24" s="3">
+        <v>0</v>
+      </c>
+      <c r="E24" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="26" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C26" s="4"/>
-      <c r="D26" s="6">
+      <c r="C26" s="7"/>
+      <c r="D26" s="4">
         <f>SUM(D4:D23)</f>
         <v>0</v>
       </c>
-      <c r="E26" s="6">
+      <c r="E26" s="4">
         <f>SUM(E4:E24)</f>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C27" s="4"/>
-      <c r="D27" s="6">
+      <c r="C27" s="7"/>
+      <c r="D27" s="4">
         <f>(D26+E26)/2</f>
         <v>0</v>
       </c>
-      <c r="E27" s="6">
+      <c r="E27" s="4">
         <f>(D26+E26)/2</f>
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B28" s="3"/>
-      <c r="C28" s="7" t="s">
+      <c r="B28" s="2"/>
+      <c r="C28" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D28" s="6">
+      <c r="D28" s="4">
         <f>IF((D27-D26) &lt;= 0, 0, (D27-D26))</f>
         <v>0</v>
       </c>
-      <c r="E28" s="6">
+      <c r="E28" s="4">
         <f>IF((E27-E26) &lt;= 0, 0, (E27-E26))</f>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B29" s="3"/>
-      <c r="C29" s="7" t="s">
+      <c r="B29" s="2"/>
+      <c r="C29" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D29" s="6">
+      <c r="D29" s="4">
         <f>IF((D27-D26) &lt;= 0, (D26-D27), 0 )</f>
         <v>0</v>
       </c>
-      <c r="E29" s="6">
+      <c r="E29" s="4">
         <f>IF((E27-E26) &lt;= 0, (E26-E27), 0 )</f>
         <v>0</v>
       </c>
@@ -1433,18 +2215,33 @@
     <mergeCell ref="B27:C27"/>
   </mergeCells>
   <conditionalFormatting sqref="D28">
-    <cfRule type="cellIs" dxfId="2" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="27" priority="10" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D28:E28">
-    <cfRule type="cellIs" dxfId="1" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="26" priority="9" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D29:E29">
-    <cfRule type="cellIs" dxfId="0" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="25" priority="8" operator="greaterThan">
       <formula>18.55</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D4:E24">
+    <cfRule type="cellIs" dxfId="24" priority="3" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4:B24">
+    <cfRule type="cellIs" dxfId="23" priority="2" operator="equal">
+      <formula>"indicar fecha"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C4:C24">
+    <cfRule type="cellIs" dxfId="17" priority="1" operator="equal">
+      <formula>"indicar gasto"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1503,15 +2300,15 @@
       <c r="C4" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="3">
         <f>'Gastos Cristian-Cristina-Ruben'!D27</f>
         <v>150</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="3">
         <f>'Gastos Cristian-Cristina-Ruben'!E27</f>
         <v>150</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="3">
         <f>'Gastos Cristian-Cristina-Ruben'!F27</f>
         <v>150</v>
       </c>
@@ -1523,15 +2320,15 @@
       <c r="C5" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="3">
         <f>'Gastos Cristian-Cristina'!D27</f>
         <v>0</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="3">
         <f>'Gastos Cristian-Cristina'!E27</f>
         <v>0</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="3">
         <v>0</v>
       </c>
     </row>
@@ -1542,100 +2339,100 @@
       <c r="C6" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="5">
-        <v>0</v>
-      </c>
-      <c r="E6" s="5">
+      <c r="D6" s="3">
+        <v>0</v>
+      </c>
+      <c r="E6" s="3">
         <f>'Gastos Cristina-Ruben'!D27</f>
         <v>0</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="3">
         <f>'Gastos Cristina-Ruben'!E27</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B7" s="1"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
     </row>
     <row r="8" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="11">
+      <c r="C8" s="11"/>
+      <c r="D8" s="6">
         <f>SUM(D4:D6)</f>
         <v>150</v>
       </c>
-      <c r="E8" s="11">
+      <c r="E8" s="6">
         <f>SUM(E4:E6)</f>
         <v>150</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="6">
         <f>SUM(F4:F6)</f>
         <v>150</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B14" s="1"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B15" s="1"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B16" s="1"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" s="1"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" s="1"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" s="1"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" s="1"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B22" s="1"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B23" s="1"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B24" s="1"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B25" s="1"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>